<commit_message>
Added Gender Filter, finished Initialize.java.
</commit_message>
<xml_diff>
--- a/src/main/resources/roommateSheet.xlsx
+++ b/src/main/resources/roommateSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Java\roommateMatching\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D31B16-11CB-4EEB-9376-635EA0001FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBCCDC9-9E00-49FF-AA55-AA9FF818EAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>Id</t>
   </si>
@@ -152,41 +152,50 @@
     <t>abc3de</t>
   </si>
   <si>
+    <t>Drake Sullivan</t>
+  </si>
+  <si>
+    <t>lbt4ba</t>
+  </si>
+  <si>
+    <t>Second Choice</t>
+  </si>
+  <si>
+    <t>Night Owl</t>
+  </si>
+  <si>
+    <t>I can not use my legs.</t>
+  </si>
+  <si>
+    <t>trq4ab</t>
+  </si>
+  <si>
+    <t>Sara Kolsan</t>
+  </si>
+  <si>
+    <t>qeb7ty</t>
+  </si>
+  <si>
+    <t>Which Gender would you like to room with?</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Ayla Smith</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>Drake Sullivan</t>
-  </si>
-  <si>
-    <t>lbt4ba</t>
-  </si>
-  <si>
-    <t>Second Choice</t>
-  </si>
-  <si>
-    <t>Night Owl</t>
-  </si>
-  <si>
-    <t>I can not use my legs.</t>
-  </si>
-  <si>
-    <t>Tyree Smith</t>
-  </si>
-  <si>
-    <t>trq4ab</t>
-  </si>
-  <si>
-    <t>Sara Kolsan</t>
-  </si>
-  <si>
-    <t>qeb7ty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,13 +203,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FF5B9BD5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -215,89 +251,140 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDEBF7"/>
+          <bgColor rgb="FFDDEBF7"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDEBF7"/>
+          <bgColor rgb="FFDDEBF7"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDEBF7"/>
+          <bgColor rgb="FFDDEBF7"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDEBF7"/>
+          <bgColor rgb="FFDDEBF7"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDEBF7"/>
+          <bgColor rgb="FFDDEBF7"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -319,10 +406,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:AC6" totalsRowShown="0">
-  <autoFilter ref="A1:AC6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="29">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:AD6" totalsRowShown="0">
+  <autoFilter ref="A1:AD6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="30">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="6">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="id"/>
@@ -343,188 +430,165 @@
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="25">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="5">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="responder"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="24">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="responderName"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Full Name" dataDxfId="23">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="r1edc3fc2615645be90aea1714fe00253"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Computing ID" dataDxfId="22">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="r41c3b28ca86b4edd9015933bb79d2b64"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Please indicate the total number of people you wish to have in a group. Include yourself..4" dataDxfId="21">
-      <extLst>
-        <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
-          <xlmsforms:question id="r48a32ba545984782bc2d834d69ecaca2"/>
-        </ext>
-      </extLst>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Please indicate the total number of people you wish to have in a group. Include yourself..2" dataDxfId="20">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Name">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="ree2f127ae997463aa3139e6b41a0a7ee"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="In the event that we can only find matches that are less than 50% compatible for your first group preference, would you rather we switch to your secondary preference?" dataDxfId="19">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Full Name">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r45d201031e384ab8973a440437159b81"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="How many roommates are in your current group?" dataDxfId="18">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Computing ID">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r54f5b46138a7468981c3604ebcf07c05"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Out of 5, select how clean you keep shared living spaces on average. (1 = disorganized, 5 = virtually spotless)" dataDxfId="17">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Which Gender would you like to room with?">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rc053dc60cdaa43f59d9d8eafd4e1d69c"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Out of 5, select the lowest amount of stars you would be comfortable with for your roommate(s)'s cleaning habits. (1 = disorganized, 5 = virtually spotless)" dataDxfId="16">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Please indicate the total number of people you wish to have in a group. Include yourself..4">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r76ec996a43fa4569a848f7fcdc5fb1d4"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Out of 5, how much importance does the topic of cleanliness matter to your match selection? (1 = not at all, 5 = extremely important)" dataDxfId="15">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Please indicate the total number of people you wish to have in a group. Include yourself..2">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r5416490c467a4be886fcb98fd47f5f05"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Out of 5, select how much you plan to bring outside guests to your living space (1 = almost never, 5 = almost everyday)" dataDxfId="14">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="In the event that we can only find matches that are less than 50% compatible for your first group preference, would you rather we switch to your secondary preference?">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rf43806c4662e4a28860a707015323b36"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Out of 5, select how much you would wish your roommate(s) bring outside guests over. (1 = almost never, 5 = almost everyday)" dataDxfId="13">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="How many roommates are in your current group?">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r9189dc6f188f46e3adf73ce94e3b73b8"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Out of 5, how much importance does the topic of having outside guests matter to your match selection? (1 = not at all, 5 = extremely important)" dataDxfId="12">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Out of 5, select how clean you keep shared living spaces on average. (1 = disorganized, 5 = virtually spotless)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r78f78f30651b4040818cbb379d888b5e"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Out of 5, select how often you wish to hang out with your roommate(s) (1 = very rarely, 5 = quite often)" dataDxfId="11">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Out of 5, select the lowest amount of stars you would be comfortable with for your roommate(s)'s cleaning habits. (1 = disorganized, 5 = virtually spotless)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r51420aca9b94412098bf8348837c1d29"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Out of 5, how much importance does the topic of hanging out with roommate(s) to your match selection? (1 = not at all, 5 = extremely important)" dataDxfId="10">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Out of 5, how much importance does the topic of cleanliness matter to your match selection? (1 = not at all, 5 = extremely important)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="reee90cae41dd4f24b5292d46835113bd"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Which of the following do you most likely consider yourself regard sleep schedule?" dataDxfId="9">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Out of 5, select how much you plan to bring outside guests to your living space (1 = almost never, 5 = almost everyday)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rc5fefecb26b44cb093503f55a9281f06"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Out of 5, how much importance does the topic of sharing a similar sleep schedule have for your match selection? (1 = not at all, 5 = extremely important)" dataDxfId="8">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Out of 5, select how much you would wish your roommate(s) bring outside guests over. (1 = almost never, 5 = almost everyday)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rad69a36b0fd74b1c957be1db441bb746"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="On a scale of 1 to 5, how extroverted are you? (1 = very introverted, 5 = very extroverted)" dataDxfId="7">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Out of 5, how much importance does the topic of having outside guests matter to your match selection? (1 = not at all, 5 = extremely important)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rf4f66b6563d641a78e788dc97cd77f98"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="On a scale of 1 to 5, how extroverted would you prefer your roommate(s) to be? (1 = very introverted, 2 = very extroverted)" dataDxfId="6">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Out of 5, select how often you wish to hang out with your roommate(s) (1 = very rarely, 5 = quite often)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="re51684996b9645c792fb889feab58f3d"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Out of 5, how much importance does the topic of personality type have for your match selection? (1 = not at all, 5 = extremely important)" dataDxfId="5">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Out of 5, how much importance does the topic of hanging out with roommate(s) to your match selection? (1 = not at all, 5 = extremely important)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r2a9bea376edd45ea88f699b61e8d50db"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="On a scale of 1 to 5, how often do you think you will be present at your living space on a daily basis? (1 = almost never, 5 = almost always)" dataDxfId="4">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Which of the following do you most likely consider yourself regard sleep schedule?">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r17766bca789a483482de886248fdcfd8"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Out of 5, how much would you prefer your roommate(s) to be in your shared living space? (1 = almost never, 5 = almost always)" dataDxfId="3">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Out of 5, how much importance does the topic of sharing a similar sleep schedule have for your match selection? (1 = not at all, 5 = extremely important)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="r88cca55575e74b36b66e15896f39f117"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Out of 5, how much importance does the topic of roommate(s) presence have for your match selection? (1 = not at all, 5 = extremely important)" dataDxfId="2">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="On a scale of 1 to 5, how extroverted are you? (1 = very introverted, 5 = very extroverted)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="ra8e7d8ff64d54e1f8447a42510d72662"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Are there any special religious traditions and/or rules that need to be considered when matching? (i.e. Lent, Ramadan, Kosher, etc.)" dataDxfId="1">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="On a scale of 1 to 5, how extroverted would you prefer your roommate(s) to be? (1 = very introverted, 2 = very extroverted)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="red87fade482a43d7a90b7b1a98162ad6"/>
         </ext>
       </extLst>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Please leave any information or special requests here:" dataDxfId="0">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Out of 5, how much importance does the topic of personality type have for your match selection? (1 = not at all, 5 = extremely important)">
       <extLst>
         <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{FCC71383-01E1-4257-9335-427F07BE8D7F}">
           <xlmsforms:question id="rf49d660fdf1e4c07bc1795431209acd0"/>
         </ext>
       </extLst>
     </tableColumn>
+    <tableColumn id="30" xr3:uid="{773E401A-6B4A-43D5-935E-69CF22E3490F}" name="On a scale of 1 to 5, how often do you think you will be present at your living space on a daily basis? (1 = almost never, 5 = almost always)" dataDxfId="4"/>
+    <tableColumn id="31" xr3:uid="{78E5F79A-2FF7-4F3A-ACBD-88103F6465D2}" name="Out of 5, how much would you prefer your roommate(s) to be in your shared living space? (1 = almost never, 5 = almost always)" dataDxfId="3"/>
+    <tableColumn id="32" xr3:uid="{43C053A8-96AA-4109-856A-143290258422}" name="Out of 5, how much importance does the topic of roommate(s) presence have for your match selection? (1 = not at all, 5 = extremely important)" dataDxfId="2"/>
+    <tableColumn id="33" xr3:uid="{25855648-4C24-420A-AFE1-ACED26CBAA68}" name="Are there any special religious traditions and/or rules that need to be considered when matching? (i.e. Lent, Ramadan, Kosher, etc.)" dataDxfId="1"/>
+    <tableColumn id="34" xr3:uid="{962211FB-F9EE-4956-A5FA-A078575D0EE6}" name="Please leave any information or special requests here:" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -862,18 +926,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="29" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="25" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:30" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -886,469 +950,506 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>45067.989594907405</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>45067.991030092591</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L2">
-        <v>4</v>
-      </c>
-      <c r="M2">
-        <v>3</v>
-      </c>
-      <c r="N2">
+      <c r="M2" s="4">
+        <v>4</v>
+      </c>
+      <c r="N2" s="4">
+        <v>3</v>
+      </c>
+      <c r="O2" s="4">
         <v>5</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
+      <c r="P2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="4">
         <v>2</v>
       </c>
-      <c r="Q2">
-        <v>3</v>
-      </c>
-      <c r="R2">
-        <v>3</v>
-      </c>
-      <c r="S2">
-        <v>3</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="R2" s="4">
+        <v>3</v>
+      </c>
+      <c r="S2" s="4">
+        <v>3</v>
+      </c>
+      <c r="T2" s="4">
+        <v>3</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>3</v>
-      </c>
-      <c r="W2">
-        <v>3</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2">
-        <v>4</v>
-      </c>
-      <c r="Z2">
-        <v>3</v>
-      </c>
-      <c r="AA2">
-        <v>3</v>
-      </c>
+      <c r="V2" s="4">
+        <v>1</v>
+      </c>
+      <c r="W2" s="4">
+        <v>3</v>
+      </c>
+      <c r="X2" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>45069.840474537035</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>45069.842962962961</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3">
-        <v>3</v>
-      </c>
-      <c r="M3">
+      <c r="K3" s="5"/>
+      <c r="L3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="5">
+        <v>3</v>
+      </c>
+      <c r="N3" s="5">
         <v>2</v>
       </c>
-      <c r="N3">
-        <v>3</v>
-      </c>
-      <c r="O3">
-        <v>4</v>
-      </c>
-      <c r="P3">
+      <c r="O3" s="5">
+        <v>3</v>
+      </c>
+      <c r="P3" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="5">
         <v>5</v>
       </c>
-      <c r="Q3">
-        <v>4</v>
-      </c>
-      <c r="R3">
-        <v>3</v>
-      </c>
-      <c r="S3">
-        <v>4</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="R3" s="5">
+        <v>4</v>
+      </c>
+      <c r="S3" s="5">
+        <v>3</v>
+      </c>
+      <c r="T3" s="5">
+        <v>4</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
-      <c r="V3">
-        <v>4</v>
-      </c>
-      <c r="W3">
-        <v>3</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <v>3</v>
-      </c>
-      <c r="Z3">
+      <c r="V3" s="5">
+        <v>1</v>
+      </c>
+      <c r="W3" s="5">
+        <v>4</v>
+      </c>
+      <c r="X3" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="5">
         <v>2</v>
       </c>
-      <c r="AA3">
+      <c r="AB3" s="5">
         <v>5</v>
       </c>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>45071.590219907404</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>45071.592951388891</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="4">
+        <v>5</v>
+      </c>
+      <c r="N4" s="4">
+        <v>4</v>
+      </c>
+      <c r="O4" s="4">
+        <v>4</v>
+      </c>
+      <c r="P4" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>5</v>
+      </c>
+      <c r="R4" s="4">
+        <v>1</v>
+      </c>
+      <c r="S4" s="4">
+        <v>1</v>
+      </c>
+      <c r="T4" s="4">
+        <v>1</v>
+      </c>
+      <c r="U4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4">
+      <c r="V4" s="4">
+        <v>3</v>
+      </c>
+      <c r="W4" s="4">
+        <v>2</v>
+      </c>
+      <c r="X4" s="4">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="4">
         <v>5</v>
       </c>
-      <c r="M4">
-        <v>4</v>
-      </c>
-      <c r="N4">
-        <v>4</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4">
-        <v>5</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="AB4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="U4">
-        <v>3</v>
-      </c>
-      <c r="V4">
-        <v>2</v>
-      </c>
-      <c r="W4">
-        <v>4</v>
-      </c>
-      <c r="X4">
-        <v>1</v>
-      </c>
-      <c r="Y4">
-        <v>3</v>
-      </c>
-      <c r="Z4">
-        <v>5</v>
-      </c>
-      <c r="AA4">
-        <v>1</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>45071.646689814814</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>45071.648854166669</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L5">
-        <v>3</v>
-      </c>
-      <c r="M5">
-        <v>4</v>
-      </c>
-      <c r="N5">
+      <c r="M5" s="5">
+        <v>3</v>
+      </c>
+      <c r="N5" s="5">
+        <v>4</v>
+      </c>
+      <c r="O5" s="5">
         <v>5</v>
       </c>
-      <c r="O5">
+      <c r="P5" s="5">
         <v>2</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>3</v>
-      </c>
-      <c r="R5">
-        <v>3</v>
-      </c>
-      <c r="S5">
-        <v>3</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="Q5" s="5">
+        <v>1</v>
+      </c>
+      <c r="R5" s="5">
+        <v>3</v>
+      </c>
+      <c r="S5" s="5">
+        <v>3</v>
+      </c>
+      <c r="T5" s="5">
+        <v>3</v>
+      </c>
+      <c r="U5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="U5">
-        <v>1</v>
-      </c>
-      <c r="V5">
-        <v>3</v>
-      </c>
-      <c r="W5">
-        <v>3</v>
-      </c>
-      <c r="X5">
-        <v>1</v>
-      </c>
-      <c r="Y5">
-        <v>3</v>
-      </c>
-      <c r="Z5">
-        <v>4</v>
-      </c>
-      <c r="AA5">
-        <v>3</v>
-      </c>
+      <c r="V5" s="5">
+        <v>1</v>
+      </c>
+      <c r="W5" s="5">
+        <v>3</v>
+      </c>
+      <c r="X5" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>45071.915520833332</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>45071.91978009259</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="4">
+        <v>4</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2</v>
+      </c>
+      <c r="O6" s="4">
+        <v>3</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>3</v>
+      </c>
+      <c r="R6" s="4">
+        <v>1</v>
+      </c>
+      <c r="S6" s="4">
+        <v>2</v>
+      </c>
+      <c r="T6" s="4">
+        <v>1</v>
+      </c>
+      <c r="U6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="M6">
+      <c r="V6" s="4">
+        <v>4</v>
+      </c>
+      <c r="W6" s="4">
         <v>2</v>
       </c>
-      <c r="N6">
-        <v>3</v>
-      </c>
-      <c r="O6">
+      <c r="X6" s="4">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="4">
+        <v>4</v>
+      </c>
+      <c r="AA6" s="4">
         <v>2</v>
       </c>
-      <c r="P6">
-        <v>3</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>2</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
-        <v>42</v>
-      </c>
-      <c r="U6">
-        <v>4</v>
-      </c>
-      <c r="V6">
-        <v>2</v>
-      </c>
-      <c r="W6">
-        <v>4</v>
-      </c>
-      <c r="X6">
-        <v>3</v>
-      </c>
-      <c r="Y6">
-        <v>4</v>
-      </c>
-      <c r="Z6">
-        <v>2</v>
-      </c>
-      <c r="AA6">
-        <v>4</v>
-      </c>
+      <c r="AB6" s="4">
+        <v>4</v>
+      </c>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added consideration for people with roommates when adding to Group.
</commit_message>
<xml_diff>
--- a/src/main/resources/roommateSheet.xlsx
+++ b/src/main/resources/roommateSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Java\roommateMatching\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBCCDC9-9E00-49FF-AA55-AA9FF818EAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE59F37-69E6-41DC-BF53-AF96172F0FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -186,9 +186,6 @@
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -928,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1143,8 +1140,8 @@
         <v>33</v>
       </c>
       <c r="K3" s="5"/>
-      <c r="L3" s="6" t="s">
-        <v>50</v>
+      <c r="L3" s="6">
+        <v>1</v>
       </c>
       <c r="M3" s="5">
         <v>3</v>

</xml_diff>

<commit_message>
Finished Algorithm. Beta version needs testing and edge case handling.
</commit_message>
<xml_diff>
--- a/src/main/resources/roommateSheet.xlsx
+++ b/src/main/resources/roommateSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Java\roommateMatching\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE59F37-69E6-41DC-BF53-AF96172F0FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A7C5B4-9787-474D-A1A7-745409E7E762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,9 +128,6 @@
     <t>anonymous</t>
   </si>
   <si>
-    <t>test_1</t>
-  </si>
-  <si>
     <t>tbh7cm</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>Chris Joseph</t>
   </si>
 </sst>
 </file>
@@ -926,7 +926,7 @@
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -957,7 +957,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -1041,23 +1041,23 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2" s="4">
         <v>4</v>
@@ -1084,7 +1084,7 @@
         <v>3</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V2" s="4">
         <v>1</v>
@@ -1125,19 +1125,19 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="H3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="6">
@@ -1168,7 +1168,7 @@
         <v>4</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V3" s="5">
         <v>1</v>
@@ -1209,23 +1209,23 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M4" s="4">
         <v>5</v>
@@ -1252,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V4" s="4">
         <v>3</v>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.75">
@@ -1295,23 +1295,23 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M5" s="5">
         <v>3</v>
@@ -1338,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V5" s="5">
         <v>1</v>
@@ -1379,23 +1379,23 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M6" s="4">
         <v>4</v>
@@ -1422,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V6" s="4">
         <v>4</v>

</xml_diff>

<commit_message>
Added Testing. Slight bug fixes.
</commit_message>
<xml_diff>
--- a/src/main/resources/roommateSheet.xlsx
+++ b/src/main/resources/roommateSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Java\roommateMatching\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A7C5B4-9787-474D-A1A7-745409E7E762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C149CB-AE2C-42FD-87DD-EC6ADDB11C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
   <si>
     <t>Id</t>
   </si>
@@ -186,6 +186,33 @@
   </si>
   <si>
     <t>Chris Joseph</t>
+  </si>
+  <si>
+    <t>Nikita Joy</t>
+  </si>
+  <si>
+    <t>trj2bx</t>
+  </si>
+  <si>
+    <t>Catherine Hernandez</t>
+  </si>
+  <si>
+    <t>rbx9dc</t>
+  </si>
+  <si>
+    <t>Early Bird</t>
+  </si>
+  <si>
+    <t>Hunter Smith</t>
+  </si>
+  <si>
+    <t>yuh4aw</t>
+  </si>
+  <si>
+    <t>Jackson Travis</t>
+  </si>
+  <si>
+    <t>reb4nj</t>
   </si>
 </sst>
 </file>
@@ -248,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -258,6 +285,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,8 +431,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:AD6" totalsRowShown="0">
-  <autoFilter ref="A1:AD6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:AD10" totalsRowShown="0">
+  <autoFilter ref="A1:AD10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="6">
       <extLst>
@@ -923,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1053,7 +1081,7 @@
         <v>31</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="s">
@@ -1447,6 +1475,334 @@
       </c>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45072.915520775467</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45072.919780034725</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4">
+        <v>4</v>
+      </c>
+      <c r="N7" s="4">
+        <v>3</v>
+      </c>
+      <c r="O7" s="4">
+        <v>5</v>
+      </c>
+      <c r="P7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>2</v>
+      </c>
+      <c r="R7" s="4">
+        <v>3</v>
+      </c>
+      <c r="S7" s="4">
+        <v>3</v>
+      </c>
+      <c r="T7" s="4">
+        <v>3</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" s="4">
+        <v>1</v>
+      </c>
+      <c r="W7" s="4">
+        <v>4</v>
+      </c>
+      <c r="X7" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>4</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45073.915520775467</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45072.919780034725</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4">
+        <v>5</v>
+      </c>
+      <c r="N8" s="4">
+        <v>3</v>
+      </c>
+      <c r="O8" s="4">
+        <v>5</v>
+      </c>
+      <c r="P8" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>2</v>
+      </c>
+      <c r="R8" s="4">
+        <v>2</v>
+      </c>
+      <c r="S8" s="4">
+        <v>3</v>
+      </c>
+      <c r="T8" s="4">
+        <v>3</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" s="4">
+        <v>1</v>
+      </c>
+      <c r="W8" s="4">
+        <v>3</v>
+      </c>
+      <c r="X8" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>4</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45073.915520775467</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45072.919780034725</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="4">
+        <v>5</v>
+      </c>
+      <c r="N9" s="4">
+        <v>3</v>
+      </c>
+      <c r="O9" s="4">
+        <v>5</v>
+      </c>
+      <c r="P9" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>2</v>
+      </c>
+      <c r="R9" s="4">
+        <v>2</v>
+      </c>
+      <c r="S9" s="4">
+        <v>3</v>
+      </c>
+      <c r="T9" s="4">
+        <v>3</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V9" s="4">
+        <v>1</v>
+      </c>
+      <c r="W9" s="4">
+        <v>3</v>
+      </c>
+      <c r="X9" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>4</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45073.915520775467</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45072.919780034725</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="4">
+        <v>5</v>
+      </c>
+      <c r="N10" s="4">
+        <v>3</v>
+      </c>
+      <c r="O10" s="4">
+        <v>5</v>
+      </c>
+      <c r="P10" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>2</v>
+      </c>
+      <c r="R10" s="4">
+        <v>2</v>
+      </c>
+      <c r="S10" s="4">
+        <v>3</v>
+      </c>
+      <c r="T10" s="4">
+        <v>3</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V10" s="4">
+        <v>1</v>
+      </c>
+      <c r="W10" s="4">
+        <v>3</v>
+      </c>
+      <c r="X10" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>4</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB10" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>